<commit_message>
change import file to student
</commit_message>
<xml_diff>
--- a/public/download/import_student_example.xlsx
+++ b/public/download/import_student_example.xlsx
@@ -16,117 +16,201 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
-  <si>
-    <t>Batch name</t>
-  </si>
-  <si>
-    <t>Admission no</t>
-  </si>
-  <si>
-    <t>Student name</t>
-  </si>
-  <si>
-    <t>Admission date</t>
-  </si>
-  <si>
-    <t>Date of birth</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="65">
   <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>Nationality</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
     <t>State</t>
   </si>
   <si>
-    <t>Pin code</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
     <t>Mobile</t>
   </si>
   <si>
-    <t>Immediate contact</t>
-  </si>
-  <si>
-    <t>Biometric</t>
-  </si>
-  <si>
-    <t>All siblings</t>
-  </si>
-  <si>
-    <t>G10 - 2015-16-T1</t>
-  </si>
-  <si>
-    <t>Bajwa Gurseerat  Singh</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>With Sibling</t>
   </si>
   <si>
-    <t xml:space="preserve">37 Twisted Oak Street </t>
-  </si>
-  <si>
     <t>Brampton</t>
   </si>
   <si>
     <t>Ontario</t>
   </si>
   <si>
-    <t>L6R 1T1</t>
-  </si>
-  <si>
-    <t>(905) 792-2694</t>
-  </si>
-  <si>
-    <t>416-731-4571</t>
-  </si>
-  <si>
-    <t>Gurpersad Singh Bajwa(416-731-4571)</t>
-  </si>
-  <si>
-    <t>Bassi Simran Kaur</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
-    <t xml:space="preserve">1 Dalla Riva Crt. </t>
-  </si>
-  <si>
-    <t>L6P 0S7</t>
-  </si>
-  <si>
-    <t>(905) 794-6041</t>
-  </si>
-  <si>
-    <t>416-662-1224</t>
-  </si>
-  <si>
-    <t>Harvinder Singh Bassi(416-662-1224)</t>
+    <t>Sl. no.</t>
+  </si>
+  <si>
+    <t>Admission Date</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Address Line 1</t>
+  </si>
+  <si>
+    <t>Pin Code</t>
+  </si>
+  <si>
+    <t>Immediate contact first name</t>
+  </si>
+  <si>
+    <t>Immediate contact last name</t>
+  </si>
+  <si>
+    <t>Immediate contact relation</t>
+  </si>
+  <si>
+    <t>Immediate contact office address 1</t>
+  </si>
+  <si>
+    <t>Immediate contact city</t>
+  </si>
+  <si>
+    <t>Immediate contact state</t>
+  </si>
+  <si>
+    <t>Immediate contact office phone</t>
+  </si>
+  <si>
+    <t>Immediate contact mobile phone</t>
+  </si>
+  <si>
+    <t>Parents first name</t>
+  </si>
+  <si>
+    <t>Parents last name</t>
+  </si>
+  <si>
+    <t>Parents relation</t>
+  </si>
+  <si>
+    <t>Parents office address 1</t>
+  </si>
+  <si>
+    <t>Parents city</t>
+  </si>
+  <si>
+    <t>Parents state</t>
+  </si>
+  <si>
+    <t>Parents office phone</t>
+  </si>
+  <si>
+    <t>Parents mobile phone</t>
+  </si>
+  <si>
+    <t>Student category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/06/2015 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30/03/2005 </t>
+  </si>
+  <si>
+    <t>G5A - 2015-16-T1</t>
+  </si>
+  <si>
+    <t>Aggarwal</t>
+  </si>
+  <si>
+    <t>Akul</t>
+  </si>
+  <si>
+    <t>19 Lombardy Cres.</t>
+  </si>
+  <si>
+    <t>L6S 4L7</t>
+  </si>
+  <si>
+    <t>905-455-7321</t>
+  </si>
+  <si>
+    <t>647-287-7321</t>
+  </si>
+  <si>
+    <t>Kamal</t>
+  </si>
+  <si>
+    <t>father</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Renuka</t>
+  </si>
+  <si>
+    <t>mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/12/2002 </t>
+  </si>
+  <si>
+    <t>G8A - 2015-16-T1</t>
+  </si>
+  <si>
+    <t>Ishita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/04/2007 </t>
+  </si>
+  <si>
+    <t>G3B - 2015-16-T1</t>
+  </si>
+  <si>
+    <t>Ahluwalia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angad </t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>57 Pefferlaw Circle</t>
+  </si>
+  <si>
+    <t>L6Y 0L6</t>
+  </si>
+  <si>
+    <t>(905) 497-4621</t>
+  </si>
+  <si>
+    <t>416-624-9511</t>
+  </si>
+  <si>
+    <t>Harprit Singh</t>
+  </si>
+  <si>
+    <t>905-497-4621</t>
+  </si>
+  <si>
+    <t>Varinder Kaur</t>
   </si>
 </sst>
 </file>
@@ -165,7 +249,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,15 +546,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
@@ -478,163 +564,447 @@
     <col min="17" max="17" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="K1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="3" spans="1:31">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W3" t="s">
+        <v>48</v>
+      </c>
+      <c r="X3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" t="s">
+        <v>7</v>
+      </c>
+      <c r="T4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" t="s">
+        <v>43</v>
+      </c>
+      <c r="V4" t="s">
+        <v>44</v>
+      </c>
+      <c r="W4" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
+    <row r="5" spans="1:31">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="W5" t="s">
+        <v>48</v>
+      </c>
+      <c r="X5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
         <v>56</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1">
-        <v>42163</v>
-      </c>
-      <c r="E2" s="1">
-        <v>36628</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" t="s">
-        <v>29</v>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6" t="s">
+        <v>62</v>
+      </c>
+      <c r="P6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T6" t="s">
+        <v>8</v>
+      </c>
+      <c r="U6" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" t="s">
+        <v>61</v>
+      </c>
+      <c r="W6" t="s">
+        <v>62</v>
+      </c>
+      <c r="X6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>84</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1">
-        <v>42164</v>
-      </c>
-      <c r="E3" s="1">
-        <v>36757</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3">
-        <v>85</v>
+    <row r="7" spans="1:31">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="W7" t="s">
+        <v>64</v>
+      </c>
+      <c r="X7" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>